<commit_message>
Updated project data collections
</commit_message>
<xml_diff>
--- a/Templates/sample_inventory/Sample_Inventory_Metadata_2023Q1_template.xlsx
+++ b/Templates/sample_inventory/Sample_Inventory_Metadata_2023Q1_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39B72835-710F-8644-A73A-D74FCF6FB742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A5F53D-FED3-FF4B-9BAA-1C6E766AD5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="500" windowWidth="23300" windowHeight="17220" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="966">
   <si>
     <t>Sample Level Metadata:</t>
   </si>
@@ -2853,7 +2853,91 @@
     <t>BossDB</t>
   </si>
   <si>
-    <t>Changes to template for April 2023</t>
+    <t>lein_great_ape_mtg_RNA_proj</t>
+  </si>
+  <si>
+    <t>lein_great_ape_MTG_10x_chimpanzee</t>
+  </si>
+  <si>
+    <t>Chimpanzee (Pan troglodytes) middle temporal gyrus (MTG) snRNA-seq</t>
+  </si>
+  <si>
+    <t>lein_great_ape_MTG_10x_gorilla</t>
+  </si>
+  <si>
+    <t>Gorilla (Gorilla gorilla) middle temporal gyrus (MTG) snRNA-seq</t>
+  </si>
+  <si>
+    <t>lein_great_ape_MTG_10x_human</t>
+  </si>
+  <si>
+    <t>Human (Homo sapiens) middle temporal gyrus (MTG) snRNA-seq</t>
+  </si>
+  <si>
+    <t>lein_great_ape_MTG_10x_marmoset</t>
+  </si>
+  <si>
+    <t>Common marmoset (Callithrix jacchus) middle temporal gyrus (MTG) snRNA-seq</t>
+  </si>
+  <si>
+    <t>lein_great_ape_MTG_10x_rhesus</t>
+  </si>
+  <si>
+    <t>Rhesus macaque (Macaca mulatta) middle temporal gyrus (MTG) snRNA-seq</t>
+  </si>
+  <si>
+    <t>lein_great_ape_MTG_SSv4_chimpanzee</t>
+  </si>
+  <si>
+    <t>lein_great_ape_MTG_SSv4_gorilla</t>
+  </si>
+  <si>
+    <t>lein_great_ape_MTG_SSv4_human</t>
+  </si>
+  <si>
+    <t>RF1 Roussos</t>
+  </si>
+  <si>
+    <t>roussos_multiome_proj</t>
+  </si>
+  <si>
+    <t>roussos_hu_multiome_atac</t>
+  </si>
+  <si>
+    <t>10x single nucleus Multiome ATAC of the human dentate gyrus</t>
+  </si>
+  <si>
+    <t>roussos_hu_multiome_gex</t>
+  </si>
+  <si>
+    <t>10x single nucleus Multiome Gene Expression of the human dentate gyrus</t>
+  </si>
+  <si>
+    <t>roussos_hu_multiome_seqfish</t>
+  </si>
+  <si>
+    <t>seqFISH+ of the human dentate gyrus</t>
+  </si>
+  <si>
+    <t>zhangK_hu_multiome_atac</t>
+  </si>
+  <si>
+    <t>Multiome ATAC-seq data from Human Brain</t>
+  </si>
+  <si>
+    <t>zhangK_hu_multiome_gex</t>
+  </si>
+  <si>
+    <t>Multiome RNA-seq data from Human Brain</t>
+  </si>
+  <si>
+    <t>zhangK_multiome_proj</t>
+  </si>
+  <si>
+    <t>zhuang_dulac_merfish_HYP_3</t>
+  </si>
+  <si>
+    <t>Changes to template for March 2023</t>
   </si>
 </sst>
 </file>
@@ -4078,10 +4162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4091,70 +4175,73 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="9" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="10" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="12" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-    </row>
-    <row r="13" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
+    <row r="13" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="17" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="39" x14ac:dyDescent="0.45">
-      <c r="A17" s="21"/>
+    <row r="18" spans="1:1" ht="39" x14ac:dyDescent="0.45">
+      <c r="A18" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4167,7 +4254,7 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4656,7 +4743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -5613,10 +5700,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EDC583-1A24-4950-A0DA-611E0CF11932}">
-  <dimension ref="A1:G333"/>
+  <dimension ref="A1:G348"/>
   <sheetViews>
-    <sheetView topLeftCell="B104" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7011,7 +7098,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>446</v>
       </c>
@@ -7028,7 +7115,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>446</v>
       </c>
@@ -7042,7 +7129,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>446</v>
       </c>
@@ -7056,7 +7143,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>446</v>
       </c>
@@ -7070,7 +7157,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>446</v>
       </c>
@@ -7084,7 +7171,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>446</v>
       </c>
@@ -7098,7 +7185,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>446</v>
       </c>
@@ -7112,840 +7199,783 @@
         <v>543</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>446</v>
       </c>
       <c r="B88" t="s">
-        <v>544</v>
+        <v>937</v>
       </c>
       <c r="C88" s="25" t="s">
-        <v>545</v>
+        <v>938</v>
       </c>
       <c r="D88" t="s">
-        <v>546</v>
-      </c>
-      <c r="E88" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>446</v>
       </c>
       <c r="B89" t="s">
-        <v>544</v>
+        <v>937</v>
       </c>
       <c r="C89" s="25" t="s">
-        <v>548</v>
+        <v>940</v>
       </c>
       <c r="D89" t="s">
-        <v>549</v>
-      </c>
-      <c r="E89" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>446</v>
       </c>
       <c r="B90" t="s">
-        <v>544</v>
+        <v>937</v>
       </c>
       <c r="C90" s="25" t="s">
-        <v>551</v>
+        <v>942</v>
       </c>
       <c r="D90" t="s">
-        <v>552</v>
-      </c>
-      <c r="E90" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>446</v>
       </c>
       <c r="B91" t="s">
-        <v>554</v>
+        <v>937</v>
       </c>
       <c r="C91" s="25" t="s">
-        <v>555</v>
+        <v>944</v>
       </c>
       <c r="D91" t="s">
-        <v>556</v>
-      </c>
-      <c r="E91" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>446</v>
       </c>
       <c r="B92" t="s">
-        <v>554</v>
+        <v>937</v>
       </c>
       <c r="C92" s="25" t="s">
-        <v>558</v>
+        <v>946</v>
       </c>
       <c r="D92" t="s">
-        <v>559</v>
-      </c>
-      <c r="E92" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>446</v>
       </c>
       <c r="B93" t="s">
-        <v>554</v>
+        <v>937</v>
       </c>
       <c r="C93" s="25" t="s">
-        <v>561</v>
+        <v>948</v>
       </c>
       <c r="D93" t="s">
-        <v>562</v>
-      </c>
-      <c r="E93" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>446</v>
       </c>
       <c r="B94" t="s">
-        <v>564</v>
+        <v>937</v>
       </c>
       <c r="C94" s="25" t="s">
-        <v>565</v>
+        <v>949</v>
       </c>
       <c r="D94" t="s">
-        <v>566</v>
-      </c>
-      <c r="E94" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>446</v>
       </c>
       <c r="B95" t="s">
-        <v>568</v>
+        <v>937</v>
       </c>
       <c r="C95" s="25" t="s">
-        <v>569</v>
+        <v>950</v>
       </c>
       <c r="D95" t="s">
-        <v>566</v>
-      </c>
-      <c r="E95" t="s">
-        <v>570</v>
-      </c>
-      <c r="F95" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>446</v>
       </c>
       <c r="B96" t="s">
-        <v>568</v>
+        <v>544</v>
       </c>
       <c r="C96" s="25" t="s">
-        <v>572</v>
+        <v>545</v>
       </c>
       <c r="D96" t="s">
-        <v>566</v>
+        <v>546</v>
       </c>
       <c r="E96" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>446</v>
       </c>
       <c r="B97" t="s">
-        <v>573</v>
-      </c>
-      <c r="C97" s="46" t="s">
-        <v>574</v>
-      </c>
-      <c r="D97" s="47" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+        <v>544</v>
+      </c>
+      <c r="C97" s="25" t="s">
+        <v>548</v>
+      </c>
+      <c r="D97" t="s">
+        <v>549</v>
+      </c>
+      <c r="E97" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>446</v>
       </c>
       <c r="B98" t="s">
-        <v>576</v>
+        <v>544</v>
       </c>
       <c r="C98" s="25" t="s">
-        <v>577</v>
+        <v>551</v>
       </c>
       <c r="D98" t="s">
-        <v>578</v>
+        <v>552</v>
       </c>
       <c r="E98" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>446</v>
       </c>
       <c r="B99" t="s">
-        <v>576</v>
+        <v>554</v>
       </c>
       <c r="C99" s="25" t="s">
-        <v>580</v>
+        <v>555</v>
       </c>
       <c r="D99" t="s">
-        <v>581</v>
+        <v>556</v>
       </c>
       <c r="E99" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>446</v>
       </c>
       <c r="B100" t="s">
-        <v>576</v>
+        <v>554</v>
       </c>
       <c r="C100" s="25" t="s">
-        <v>583</v>
+        <v>558</v>
       </c>
       <c r="D100" t="s">
-        <v>584</v>
+        <v>559</v>
       </c>
       <c r="E100" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>446</v>
       </c>
-      <c r="B101" s="31" t="s">
+      <c r="B101" t="s">
+        <v>554</v>
+      </c>
+      <c r="C101" s="25" t="s">
+        <v>561</v>
+      </c>
+      <c r="D101" t="s">
+        <v>562</v>
+      </c>
+      <c r="E101" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>446</v>
+      </c>
+      <c r="B102" t="s">
+        <v>564</v>
+      </c>
+      <c r="C102" s="25" t="s">
+        <v>565</v>
+      </c>
+      <c r="D102" t="s">
+        <v>566</v>
+      </c>
+      <c r="E102" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>446</v>
+      </c>
+      <c r="B103" t="s">
+        <v>568</v>
+      </c>
+      <c r="C103" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="D103" t="s">
+        <v>566</v>
+      </c>
+      <c r="E103" t="s">
+        <v>570</v>
+      </c>
+      <c r="F103" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>446</v>
+      </c>
+      <c r="B104" t="s">
+        <v>568</v>
+      </c>
+      <c r="C104" s="25" t="s">
+        <v>572</v>
+      </c>
+      <c r="D104" t="s">
+        <v>566</v>
+      </c>
+      <c r="E104" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>446</v>
+      </c>
+      <c r="B105" t="s">
+        <v>573</v>
+      </c>
+      <c r="C105" s="46" t="s">
+        <v>574</v>
+      </c>
+      <c r="D105" s="47" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>446</v>
+      </c>
+      <c r="B106" t="s">
         <v>576</v>
       </c>
-      <c r="C101" s="25" t="s">
+      <c r="C106" s="25" t="s">
+        <v>577</v>
+      </c>
+      <c r="D106" t="s">
+        <v>578</v>
+      </c>
+      <c r="E106" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>446</v>
+      </c>
+      <c r="B107" t="s">
+        <v>576</v>
+      </c>
+      <c r="C107" s="25" t="s">
+        <v>580</v>
+      </c>
+      <c r="D107" t="s">
+        <v>581</v>
+      </c>
+      <c r="E107" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>446</v>
+      </c>
+      <c r="B108" t="s">
+        <v>576</v>
+      </c>
+      <c r="C108" s="25" t="s">
+        <v>583</v>
+      </c>
+      <c r="D108" t="s">
+        <v>584</v>
+      </c>
+      <c r="E108" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>446</v>
+      </c>
+      <c r="B109" s="31" t="s">
+        <v>576</v>
+      </c>
+      <c r="C109" s="25" t="s">
         <v>586</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D109" t="s">
         <v>587</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E109" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>589</v>
-      </c>
-      <c r="B102" s="31" t="s">
-        <v>590</v>
-      </c>
-      <c r="C102" s="39" t="s">
-        <v>891</v>
-      </c>
-      <c r="D102" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>589</v>
-      </c>
-      <c r="B103" s="31" t="s">
-        <v>590</v>
-      </c>
-      <c r="C103" s="39" t="s">
-        <v>892</v>
-      </c>
-      <c r="D103" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>589</v>
-      </c>
-      <c r="B104" s="31" t="s">
-        <v>590</v>
-      </c>
-      <c r="C104" s="39" t="s">
-        <v>893</v>
-      </c>
-      <c r="D104" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>589</v>
-      </c>
-      <c r="B105" s="31" t="s">
-        <v>590</v>
-      </c>
-      <c r="C105" s="39" t="s">
-        <v>894</v>
-      </c>
-      <c r="D105" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>589</v>
-      </c>
-      <c r="B106" t="s">
-        <v>591</v>
-      </c>
-      <c r="C106" s="25" t="s">
-        <v>592</v>
-      </c>
-      <c r="D106" t="s">
-        <v>593</v>
-      </c>
-      <c r="E106" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>589</v>
-      </c>
-      <c r="B107" s="31" t="s">
-        <v>595</v>
-      </c>
-      <c r="C107" s="39" t="s">
-        <v>596</v>
-      </c>
-      <c r="D107" t="s">
-        <v>597</v>
-      </c>
-      <c r="E107" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>589</v>
-      </c>
-      <c r="B108" s="31" t="s">
-        <v>595</v>
-      </c>
-      <c r="C108" s="39" t="s">
-        <v>599</v>
-      </c>
-      <c r="D108" t="s">
-        <v>600</v>
-      </c>
-      <c r="E108" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>589</v>
-      </c>
-      <c r="B109" t="s">
-        <v>595</v>
-      </c>
-      <c r="C109" s="25" t="s">
-        <v>601</v>
-      </c>
-      <c r="D109" t="s">
-        <v>602</v>
-      </c>
-      <c r="E109" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>589</v>
       </c>
-      <c r="B110" t="s">
-        <v>595</v>
-      </c>
-      <c r="C110" s="25" t="s">
-        <v>604</v>
+      <c r="B110" s="31" t="s">
+        <v>590</v>
+      </c>
+      <c r="C110" s="39" t="s">
+        <v>891</v>
       </c>
       <c r="D110" t="s">
-        <v>605</v>
-      </c>
-      <c r="E110" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>589</v>
       </c>
-      <c r="B111" t="s">
-        <v>909</v>
-      </c>
-      <c r="C111" s="25" t="s">
-        <v>910</v>
+      <c r="B111" s="31" t="s">
+        <v>590</v>
+      </c>
+      <c r="C111" s="39" t="s">
+        <v>892</v>
       </c>
       <c r="D111" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>618</v>
-      </c>
-      <c r="B112" t="s">
-        <v>918</v>
-      </c>
-      <c r="C112" s="25" t="s">
-        <v>919</v>
+        <v>589</v>
+      </c>
+      <c r="B112" s="31" t="s">
+        <v>590</v>
+      </c>
+      <c r="C112" s="39" t="s">
+        <v>893</v>
       </c>
       <c r="D112" t="s">
-        <v>920</v>
+        <v>897</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>618</v>
-      </c>
-      <c r="B113" t="s">
-        <v>619</v>
-      </c>
-      <c r="C113" s="25" t="s">
-        <v>620</v>
+        <v>589</v>
+      </c>
+      <c r="B113" s="31" t="s">
+        <v>590</v>
+      </c>
+      <c r="C113" s="39" t="s">
+        <v>894</v>
       </c>
       <c r="D113" t="s">
-        <v>621</v>
-      </c>
-      <c r="E113" t="s">
-        <v>622</v>
-      </c>
-      <c r="F113" t="s">
-        <v>623</v>
-      </c>
-      <c r="G113" t="s">
-        <v>363</v>
+        <v>898</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>624</v>
+        <v>589</v>
       </c>
       <c r="B114" t="s">
-        <v>625</v>
+        <v>591</v>
       </c>
       <c r="C114" s="25" t="s">
-        <v>912</v>
+        <v>592</v>
       </c>
       <c r="D114" t="s">
-        <v>913</v>
+        <v>593</v>
+      </c>
+      <c r="E114" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>624</v>
-      </c>
-      <c r="B115" t="s">
-        <v>625</v>
-      </c>
-      <c r="C115" s="25" t="s">
-        <v>931</v>
+        <v>589</v>
+      </c>
+      <c r="B115" s="31" t="s">
+        <v>595</v>
+      </c>
+      <c r="C115" s="39" t="s">
+        <v>596</v>
       </c>
       <c r="D115" t="s">
-        <v>932</v>
+        <v>597</v>
+      </c>
+      <c r="E115" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>624</v>
-      </c>
-      <c r="B116" t="s">
-        <v>625</v>
+        <v>589</v>
+      </c>
+      <c r="B116" s="31" t="s">
+        <v>595</v>
       </c>
       <c r="C116" s="39" t="s">
-        <v>626</v>
+        <v>599</v>
       </c>
       <c r="D116" t="s">
-        <v>627</v>
+        <v>600</v>
       </c>
       <c r="E116" t="s">
-        <v>628</v>
+        <v>598</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>624</v>
+        <v>589</v>
       </c>
       <c r="B117" t="s">
-        <v>625</v>
-      </c>
-      <c r="C117" s="39" t="s">
-        <v>629</v>
+        <v>595</v>
+      </c>
+      <c r="C117" s="25" t="s">
+        <v>601</v>
       </c>
       <c r="D117" t="s">
-        <v>627</v>
+        <v>602</v>
       </c>
       <c r="E117" t="s">
-        <v>628</v>
+        <v>603</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>624</v>
+        <v>589</v>
       </c>
       <c r="B118" t="s">
-        <v>625</v>
-      </c>
-      <c r="C118" s="39" t="s">
-        <v>630</v>
+        <v>595</v>
+      </c>
+      <c r="C118" s="25" t="s">
+        <v>604</v>
       </c>
       <c r="D118" t="s">
-        <v>631</v>
+        <v>605</v>
+      </c>
+      <c r="E118" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>624</v>
+        <v>589</v>
       </c>
       <c r="B119" t="s">
-        <v>625</v>
-      </c>
-      <c r="C119" s="39" t="s">
-        <v>632</v>
+        <v>909</v>
+      </c>
+      <c r="C119" s="25" t="s">
+        <v>910</v>
       </c>
       <c r="D119" t="s">
-        <v>633</v>
-      </c>
-      <c r="E119" t="s">
-        <v>634</v>
+        <v>911</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B120" t="s">
-        <v>625</v>
-      </c>
-      <c r="C120" s="39" t="s">
-        <v>635</v>
+        <v>918</v>
+      </c>
+      <c r="C120" s="25" t="s">
+        <v>919</v>
       </c>
       <c r="D120" t="s">
-        <v>633</v>
-      </c>
-      <c r="E120" t="s">
-        <v>634</v>
+        <v>920</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B121" t="s">
-        <v>625</v>
-      </c>
-      <c r="C121" s="43" t="s">
-        <v>636</v>
-      </c>
-      <c r="D121" s="42" t="s">
-        <v>637</v>
+        <v>619</v>
+      </c>
+      <c r="C121" s="25" t="s">
+        <v>620</v>
+      </c>
+      <c r="D121" t="s">
+        <v>621</v>
+      </c>
+      <c r="E121" t="s">
+        <v>622</v>
+      </c>
+      <c r="F121" t="s">
+        <v>623</v>
+      </c>
+      <c r="G121" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>624</v>
+        <v>951</v>
       </c>
       <c r="B122" t="s">
-        <v>625</v>
-      </c>
-      <c r="C122" s="39" t="s">
-        <v>638</v>
+        <v>952</v>
+      </c>
+      <c r="C122" s="25" t="s">
+        <v>953</v>
       </c>
       <c r="D122" t="s">
-        <v>639</v>
-      </c>
-      <c r="E122" t="s">
-        <v>640</v>
+        <v>954</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>611</v>
+        <v>951</v>
       </c>
       <c r="B123" t="s">
-        <v>612</v>
+        <v>952</v>
       </c>
       <c r="C123" s="25" t="s">
-        <v>613</v>
+        <v>955</v>
       </c>
       <c r="D123" t="s">
-        <v>614</v>
-      </c>
-      <c r="E123" t="s">
-        <v>615</v>
+        <v>956</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>611</v>
+        <v>951</v>
       </c>
       <c r="B124" t="s">
-        <v>612</v>
+        <v>952</v>
       </c>
       <c r="C124" s="25" t="s">
-        <v>616</v>
+        <v>957</v>
       </c>
       <c r="D124" t="s">
-        <v>614</v>
-      </c>
-      <c r="E124" t="s">
-        <v>617</v>
+        <v>958</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>641</v>
+        <v>624</v>
       </c>
       <c r="B125" t="s">
-        <v>642</v>
+        <v>625</v>
       </c>
       <c r="C125" s="25" t="s">
-        <v>643</v>
+        <v>912</v>
       </c>
       <c r="D125" t="s">
-        <v>644</v>
-      </c>
-      <c r="E125" t="s">
-        <v>645</v>
-      </c>
-      <c r="F125" t="s">
-        <v>646</v>
-      </c>
-      <c r="G125" t="s">
-        <v>363</v>
+        <v>913</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>641</v>
+        <v>624</v>
       </c>
       <c r="B126" t="s">
-        <v>642</v>
+        <v>625</v>
       </c>
       <c r="C126" s="25" t="s">
-        <v>647</v>
+        <v>931</v>
       </c>
       <c r="D126" t="s">
-        <v>648</v>
-      </c>
-      <c r="E126" t="s">
-        <v>649</v>
+        <v>932</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
       <c r="B127" t="s">
-        <v>933</v>
-      </c>
-      <c r="C127" s="25" t="s">
-        <v>934</v>
+        <v>625</v>
+      </c>
+      <c r="C127" s="39" t="s">
+        <v>626</v>
       </c>
       <c r="D127" t="s">
-        <v>935</v>
+        <v>627</v>
+      </c>
+      <c r="E127" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
       <c r="B128" t="s">
-        <v>651</v>
-      </c>
-      <c r="C128" s="25" t="s">
-        <v>652</v>
+        <v>625</v>
+      </c>
+      <c r="C128" s="39" t="s">
+        <v>629</v>
       </c>
       <c r="D128" t="s">
-        <v>653</v>
+        <v>627</v>
       </c>
       <c r="E128" t="s">
-        <v>654</v>
-      </c>
-      <c r="G128" t="s">
-        <v>363</v>
+        <v>628</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
       <c r="B129" t="s">
-        <v>651</v>
-      </c>
-      <c r="C129" s="25" t="s">
-        <v>655</v>
+        <v>625</v>
+      </c>
+      <c r="C129" s="39" t="s">
+        <v>630</v>
       </c>
       <c r="D129" t="s">
-        <v>653</v>
-      </c>
-      <c r="E129" t="s">
-        <v>656</v>
-      </c>
-      <c r="G129" t="s">
-        <v>363</v>
+        <v>631</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
       <c r="B130" t="s">
-        <v>651</v>
-      </c>
-      <c r="C130" s="25" t="s">
-        <v>657</v>
+        <v>625</v>
+      </c>
+      <c r="C130" s="39" t="s">
+        <v>632</v>
       </c>
       <c r="D130" t="s">
-        <v>653</v>
+        <v>633</v>
       </c>
       <c r="E130" t="s">
-        <v>656</v>
-      </c>
-      <c r="G130" t="s">
-        <v>363</v>
+        <v>634</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
       <c r="B131" t="s">
-        <v>651</v>
-      </c>
-      <c r="C131" s="25" t="s">
-        <v>658</v>
+        <v>625</v>
+      </c>
+      <c r="C131" s="39" t="s">
+        <v>635</v>
       </c>
       <c r="D131" t="s">
-        <v>653</v>
+        <v>633</v>
       </c>
       <c r="E131" t="s">
-        <v>654</v>
-      </c>
-      <c r="F131" t="s">
-        <v>659</v>
-      </c>
-      <c r="G131" t="s">
-        <v>363</v>
+        <v>634</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>660</v>
+        <v>624</v>
       </c>
       <c r="B132" t="s">
-        <v>661</v>
-      </c>
-      <c r="C132" s="25" t="s">
-        <v>662</v>
-      </c>
-      <c r="D132" t="s">
-        <v>663</v>
-      </c>
-      <c r="G132" t="s">
-        <v>363</v>
+        <v>625</v>
+      </c>
+      <c r="C132" s="43" t="s">
+        <v>636</v>
+      </c>
+      <c r="D132" s="42" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>660</v>
+        <v>624</v>
       </c>
       <c r="B133" t="s">
-        <v>664</v>
-      </c>
-      <c r="C133" s="25" t="s">
-        <v>665</v>
+        <v>625</v>
+      </c>
+      <c r="C133" s="39" t="s">
+        <v>638</v>
       </c>
       <c r="D133" t="s">
-        <v>666</v>
+        <v>639</v>
       </c>
       <c r="E133" t="s">
-        <v>666</v>
+        <v>640</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>660</v>
+        <v>611</v>
       </c>
       <c r="B134" t="s">
-        <v>667</v>
+        <v>612</v>
       </c>
       <c r="C134" s="25" t="s">
-        <v>668</v>
+        <v>613</v>
       </c>
       <c r="D134" t="s">
-        <v>669</v>
+        <v>614</v>
       </c>
       <c r="E134" t="s">
-        <v>670</v>
+        <v>615</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>660</v>
+        <v>611</v>
       </c>
       <c r="B135" t="s">
-        <v>671</v>
+        <v>612</v>
       </c>
       <c r="C135" s="25" t="s">
-        <v>672</v>
+        <v>616</v>
       </c>
       <c r="D135" t="s">
-        <v>673</v>
+        <v>614</v>
       </c>
       <c r="E135" t="s">
-        <v>674</v>
-      </c>
-      <c r="F135" t="s">
-        <v>675</v>
-      </c>
-      <c r="G135" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>676</v>
+        <v>641</v>
       </c>
       <c r="B136" t="s">
-        <v>677</v>
+        <v>642</v>
       </c>
       <c r="C136" s="25" t="s">
-        <v>678</v>
+        <v>643</v>
       </c>
       <c r="D136" t="s">
-        <v>679</v>
+        <v>644</v>
       </c>
       <c r="E136" t="s">
-        <v>680</v>
+        <v>645</v>
       </c>
       <c r="F136" t="s">
-        <v>681</v>
+        <v>646</v>
       </c>
       <c r="G136" t="s">
         <v>363</v>
@@ -7953,139 +7983,118 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>676</v>
+        <v>641</v>
       </c>
       <c r="B137" t="s">
-        <v>682</v>
+        <v>642</v>
       </c>
       <c r="C137" s="25" t="s">
-        <v>683</v>
+        <v>647</v>
       </c>
       <c r="D137" t="s">
-        <v>684</v>
+        <v>648</v>
       </c>
       <c r="E137" t="s">
-        <v>685</v>
-      </c>
-      <c r="F137" t="s">
-        <v>686</v>
-      </c>
-      <c r="G137" t="s">
-        <v>363</v>
+        <v>649</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>676</v>
+        <v>650</v>
       </c>
       <c r="B138" t="s">
-        <v>687</v>
+        <v>933</v>
       </c>
       <c r="C138" s="25" t="s">
-        <v>688</v>
+        <v>934</v>
       </c>
       <c r="D138" t="s">
-        <v>689</v>
-      </c>
-      <c r="E138" t="s">
-        <v>690</v>
-      </c>
-      <c r="F138" t="s">
-        <v>691</v>
-      </c>
-      <c r="G138" t="s">
-        <v>363</v>
+        <v>935</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>676</v>
+        <v>650</v>
       </c>
       <c r="B139" t="s">
-        <v>692</v>
+        <v>963</v>
       </c>
       <c r="C139" s="25" t="s">
-        <v>693</v>
+        <v>959</v>
       </c>
       <c r="D139" t="s">
-        <v>694</v>
-      </c>
-      <c r="E139" t="s">
-        <v>695</v>
-      </c>
-      <c r="F139" t="s">
-        <v>696</v>
-      </c>
-      <c r="G139" t="s">
-        <v>363</v>
+        <v>960</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>697</v>
+        <v>650</v>
       </c>
       <c r="B140" t="s">
-        <v>698</v>
+        <v>963</v>
       </c>
       <c r="C140" s="25" t="s">
-        <v>699</v>
+        <v>961</v>
       </c>
       <c r="D140" t="s">
-        <v>700</v>
-      </c>
-      <c r="E140" t="s">
-        <v>701</v>
+        <v>962</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>697</v>
+        <v>650</v>
       </c>
       <c r="B141" t="s">
-        <v>702</v>
+        <v>651</v>
       </c>
       <c r="C141" s="25" t="s">
-        <v>703</v>
+        <v>652</v>
       </c>
       <c r="D141" t="s">
-        <v>704</v>
+        <v>653</v>
       </c>
       <c r="E141" t="s">
-        <v>705</v>
+        <v>654</v>
+      </c>
+      <c r="G141" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>697</v>
-      </c>
-      <c r="B142" s="42" t="s">
-        <v>706</v>
-      </c>
-      <c r="C142" s="43" t="s">
-        <v>707</v>
-      </c>
-      <c r="D142" s="42" t="s">
-        <v>708</v>
+        <v>650</v>
+      </c>
+      <c r="B142" t="s">
+        <v>651</v>
+      </c>
+      <c r="C142" s="25" t="s">
+        <v>655</v>
+      </c>
+      <c r="D142" t="s">
+        <v>653</v>
+      </c>
+      <c r="E142" t="s">
+        <v>656</v>
+      </c>
+      <c r="G142" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>697</v>
+        <v>650</v>
       </c>
       <c r="B143" t="s">
-        <v>709</v>
+        <v>651</v>
       </c>
       <c r="C143" s="25" t="s">
-        <v>710</v>
+        <v>657</v>
       </c>
       <c r="D143" t="s">
-        <v>711</v>
+        <v>653</v>
       </c>
       <c r="E143" t="s">
-        <v>712</v>
-      </c>
-      <c r="F143" t="s">
-        <v>713</v>
+        <v>656</v>
       </c>
       <c r="G143" t="s">
         <v>363</v>
@@ -8093,22 +8102,22 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>697</v>
+        <v>650</v>
       </c>
       <c r="B144" t="s">
-        <v>714</v>
+        <v>651</v>
       </c>
       <c r="C144" s="25" t="s">
-        <v>715</v>
+        <v>658</v>
       </c>
       <c r="D144" t="s">
-        <v>716</v>
+        <v>653</v>
       </c>
       <c r="E144" t="s">
-        <v>717</v>
+        <v>654</v>
       </c>
       <c r="F144" t="s">
-        <v>718</v>
+        <v>659</v>
       </c>
       <c r="G144" t="s">
         <v>363</v>
@@ -8116,96 +8125,96 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>697</v>
+        <v>660</v>
       </c>
       <c r="B145" t="s">
-        <v>714</v>
+        <v>661</v>
       </c>
       <c r="C145" s="25" t="s">
-        <v>719</v>
+        <v>662</v>
       </c>
       <c r="D145" t="s">
-        <v>720</v>
-      </c>
-      <c r="E145" t="s">
-        <v>721</v>
+        <v>663</v>
+      </c>
+      <c r="G145" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>697</v>
+        <v>660</v>
       </c>
       <c r="B146" t="s">
-        <v>714</v>
+        <v>664</v>
       </c>
       <c r="C146" s="25" t="s">
-        <v>722</v>
+        <v>665</v>
       </c>
       <c r="D146" t="s">
-        <v>723</v>
+        <v>666</v>
       </c>
       <c r="E146" t="s">
-        <v>724</v>
-      </c>
-      <c r="F146" t="s">
-        <v>725</v>
-      </c>
-      <c r="G146" t="s">
-        <v>363</v>
+        <v>666</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>697</v>
+        <v>660</v>
       </c>
       <c r="B147" t="s">
-        <v>726</v>
+        <v>667</v>
       </c>
       <c r="C147" s="25" t="s">
-        <v>727</v>
+        <v>668</v>
       </c>
       <c r="D147" t="s">
-        <v>728</v>
+        <v>669</v>
       </c>
       <c r="E147" t="s">
-        <v>729</v>
+        <v>670</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>697</v>
+        <v>660</v>
       </c>
       <c r="B148" t="s">
-        <v>726</v>
+        <v>671</v>
       </c>
       <c r="C148" s="25" t="s">
-        <v>730</v>
+        <v>672</v>
       </c>
       <c r="D148" t="s">
-        <v>731</v>
+        <v>673</v>
       </c>
       <c r="E148" t="s">
-        <v>732</v>
+        <v>674</v>
+      </c>
+      <c r="F148" t="s">
+        <v>675</v>
+      </c>
+      <c r="G148" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>697</v>
+        <v>676</v>
       </c>
       <c r="B149" t="s">
-        <v>733</v>
+        <v>677</v>
       </c>
       <c r="C149" s="25" t="s">
-        <v>734</v>
+        <v>678</v>
       </c>
       <c r="D149" t="s">
-        <v>735</v>
+        <v>679</v>
       </c>
       <c r="E149" t="s">
-        <v>736</v>
+        <v>680</v>
       </c>
       <c r="F149" t="s">
-        <v>737</v>
+        <v>681</v>
       </c>
       <c r="G149" t="s">
         <v>363</v>
@@ -8213,22 +8222,22 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>697</v>
+        <v>676</v>
       </c>
       <c r="B150" t="s">
-        <v>738</v>
+        <v>682</v>
       </c>
       <c r="C150" s="25" t="s">
-        <v>739</v>
+        <v>683</v>
       </c>
       <c r="D150" t="s">
-        <v>740</v>
+        <v>684</v>
       </c>
       <c r="E150" t="s">
-        <v>741</v>
+        <v>685</v>
       </c>
       <c r="F150" t="s">
-        <v>742</v>
+        <v>686</v>
       </c>
       <c r="G150" t="s">
         <v>363</v>
@@ -8236,39 +8245,45 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>697</v>
+        <v>676</v>
       </c>
       <c r="B151" t="s">
-        <v>743</v>
+        <v>687</v>
       </c>
       <c r="C151" s="25" t="s">
-        <v>744</v>
+        <v>688</v>
       </c>
       <c r="D151" t="s">
-        <v>745</v>
+        <v>689</v>
       </c>
       <c r="E151" t="s">
-        <v>746</v>
+        <v>690</v>
+      </c>
+      <c r="F151" t="s">
+        <v>691</v>
+      </c>
+      <c r="G151" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>697</v>
+        <v>676</v>
       </c>
       <c r="B152" t="s">
-        <v>747</v>
+        <v>692</v>
       </c>
       <c r="C152" s="25" t="s">
-        <v>748</v>
+        <v>693</v>
       </c>
       <c r="D152" t="s">
-        <v>749</v>
+        <v>694</v>
       </c>
       <c r="E152" t="s">
-        <v>750</v>
+        <v>695</v>
       </c>
       <c r="F152" t="s">
-        <v>751</v>
+        <v>696</v>
       </c>
       <c r="G152" t="s">
         <v>363</v>
@@ -8279,22 +8294,16 @@
         <v>697</v>
       </c>
       <c r="B153" t="s">
-        <v>752</v>
+        <v>698</v>
       </c>
       <c r="C153" s="25" t="s">
-        <v>753</v>
+        <v>699</v>
       </c>
       <c r="D153" t="s">
-        <v>754</v>
+        <v>700</v>
       </c>
       <c r="E153" t="s">
-        <v>755</v>
-      </c>
-      <c r="F153" t="s">
-        <v>756</v>
-      </c>
-      <c r="G153" t="s">
-        <v>363</v>
+        <v>701</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
@@ -8302,33 +8311,30 @@
         <v>697</v>
       </c>
       <c r="B154" t="s">
-        <v>757</v>
+        <v>702</v>
       </c>
       <c r="C154" s="25" t="s">
-        <v>758</v>
+        <v>703</v>
       </c>
       <c r="D154" t="s">
-        <v>759</v>
+        <v>704</v>
       </c>
       <c r="E154" t="s">
-        <v>759</v>
+        <v>705</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>697</v>
       </c>
-      <c r="B155" t="s">
-        <v>760</v>
-      </c>
-      <c r="C155" s="25" t="s">
-        <v>761</v>
-      </c>
-      <c r="D155" t="s">
-        <v>762</v>
-      </c>
-      <c r="E155" t="s">
-        <v>763</v>
+      <c r="B155" s="42" t="s">
+        <v>706</v>
+      </c>
+      <c r="C155" s="43" t="s">
+        <v>707</v>
+      </c>
+      <c r="D155" s="42" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
@@ -8336,16 +8342,22 @@
         <v>697</v>
       </c>
       <c r="B156" t="s">
-        <v>760</v>
+        <v>709</v>
       </c>
       <c r="C156" s="25" t="s">
-        <v>764</v>
+        <v>710</v>
       </c>
       <c r="D156" t="s">
-        <v>765</v>
+        <v>711</v>
       </c>
       <c r="E156" t="s">
-        <v>766</v>
+        <v>712</v>
+      </c>
+      <c r="F156" t="s">
+        <v>713</v>
+      </c>
+      <c r="G156" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
@@ -8353,13 +8365,22 @@
         <v>697</v>
       </c>
       <c r="B157" t="s">
-        <v>925</v>
+        <v>714</v>
       </c>
       <c r="C157" s="25" t="s">
-        <v>929</v>
+        <v>715</v>
       </c>
       <c r="D157" t="s">
-        <v>928</v>
+        <v>716</v>
+      </c>
+      <c r="E157" t="s">
+        <v>717</v>
+      </c>
+      <c r="F157" t="s">
+        <v>718</v>
+      </c>
+      <c r="G157" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
@@ -8367,13 +8388,16 @@
         <v>697</v>
       </c>
       <c r="B158" t="s">
-        <v>925</v>
-      </c>
-      <c r="C158" s="48" t="s">
-        <v>926</v>
+        <v>714</v>
+      </c>
+      <c r="C158" s="25" t="s">
+        <v>719</v>
       </c>
       <c r="D158" t="s">
-        <v>927</v>
+        <v>720</v>
+      </c>
+      <c r="E158" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
@@ -8381,13 +8405,22 @@
         <v>697</v>
       </c>
       <c r="B159" t="s">
-        <v>921</v>
+        <v>714</v>
       </c>
       <c r="C159" s="25" t="s">
-        <v>922</v>
+        <v>722</v>
       </c>
       <c r="D159" t="s">
-        <v>924</v>
+        <v>723</v>
+      </c>
+      <c r="E159" t="s">
+        <v>724</v>
+      </c>
+      <c r="F159" t="s">
+        <v>725</v>
+      </c>
+      <c r="G159" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
@@ -8395,13 +8428,16 @@
         <v>697</v>
       </c>
       <c r="B160" t="s">
-        <v>921</v>
+        <v>726</v>
       </c>
       <c r="C160" s="25" t="s">
-        <v>923</v>
+        <v>727</v>
       </c>
       <c r="D160" t="s">
-        <v>924</v>
+        <v>728</v>
+      </c>
+      <c r="E160" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
@@ -8409,16 +8445,16 @@
         <v>697</v>
       </c>
       <c r="B161" t="s">
-        <v>767</v>
+        <v>726</v>
       </c>
       <c r="C161" s="25" t="s">
-        <v>768</v>
+        <v>730</v>
       </c>
       <c r="D161" t="s">
-        <v>769</v>
+        <v>731</v>
       </c>
       <c r="E161" t="s">
-        <v>770</v>
+        <v>732</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
@@ -8426,16 +8462,22 @@
         <v>697</v>
       </c>
       <c r="B162" t="s">
-        <v>767</v>
+        <v>733</v>
       </c>
       <c r="C162" s="25" t="s">
-        <v>771</v>
+        <v>734</v>
       </c>
       <c r="D162" t="s">
-        <v>769</v>
+        <v>735</v>
       </c>
       <c r="E162" t="s">
-        <v>770</v>
+        <v>736</v>
+      </c>
+      <c r="F162" t="s">
+        <v>737</v>
+      </c>
+      <c r="G162" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
@@ -8443,16 +8485,22 @@
         <v>697</v>
       </c>
       <c r="B163" t="s">
-        <v>767</v>
+        <v>738</v>
       </c>
       <c r="C163" s="25" t="s">
-        <v>772</v>
+        <v>739</v>
       </c>
       <c r="D163" t="s">
-        <v>773</v>
+        <v>740</v>
       </c>
       <c r="E163" t="s">
-        <v>770</v>
+        <v>741</v>
+      </c>
+      <c r="F163" t="s">
+        <v>742</v>
+      </c>
+      <c r="G163" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
@@ -8460,36 +8508,36 @@
         <v>697</v>
       </c>
       <c r="B164" t="s">
-        <v>774</v>
+        <v>743</v>
       </c>
       <c r="C164" s="25" t="s">
-        <v>775</v>
+        <v>744</v>
       </c>
       <c r="D164" t="s">
-        <v>776</v>
+        <v>745</v>
       </c>
       <c r="E164" t="s">
-        <v>777</v>
+        <v>746</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B165" t="s">
-        <v>779</v>
+        <v>747</v>
       </c>
       <c r="C165" s="25" t="s">
-        <v>780</v>
+        <v>748</v>
       </c>
       <c r="D165" t="s">
-        <v>781</v>
+        <v>749</v>
       </c>
       <c r="E165" t="s">
-        <v>782</v>
+        <v>750</v>
       </c>
       <c r="F165" t="s">
-        <v>783</v>
+        <v>751</v>
       </c>
       <c r="G165" t="s">
         <v>363</v>
@@ -8497,45 +8545,36 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B166" t="s">
-        <v>779</v>
+        <v>747</v>
       </c>
       <c r="C166" s="25" t="s">
-        <v>784</v>
+        <v>710</v>
       </c>
       <c r="D166" t="s">
-        <v>785</v>
-      </c>
-      <c r="E166" t="s">
-        <v>786</v>
-      </c>
-      <c r="F166" t="s">
-        <v>787</v>
-      </c>
-      <c r="G166" t="s">
-        <v>363</v>
+        <v>711</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B167" t="s">
-        <v>779</v>
+        <v>752</v>
       </c>
       <c r="C167" s="25" t="s">
-        <v>788</v>
+        <v>753</v>
       </c>
       <c r="D167" t="s">
-        <v>789</v>
+        <v>754</v>
       </c>
       <c r="E167" t="s">
-        <v>790</v>
+        <v>755</v>
       </c>
       <c r="F167" t="s">
-        <v>791</v>
+        <v>756</v>
       </c>
       <c r="G167" t="s">
         <v>363</v>
@@ -8543,272 +8582,191 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B168" t="s">
-        <v>792</v>
+        <v>757</v>
       </c>
       <c r="C168" s="25" t="s">
-        <v>340</v>
+        <v>758</v>
       </c>
       <c r="D168" t="s">
-        <v>341</v>
+        <v>759</v>
       </c>
       <c r="E168" t="s">
-        <v>793</v>
-      </c>
-      <c r="F168" t="s">
-        <v>794</v>
-      </c>
-      <c r="G168" t="s">
-        <v>363</v>
+        <v>759</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B169" t="s">
-        <v>792</v>
+        <v>760</v>
       </c>
       <c r="C169" s="25" t="s">
-        <v>795</v>
+        <v>761</v>
       </c>
       <c r="D169" t="s">
-        <v>796</v>
+        <v>762</v>
       </c>
       <c r="E169" t="s">
-        <v>793</v>
-      </c>
-      <c r="F169" t="s">
-        <v>794</v>
-      </c>
-      <c r="G169" t="s">
-        <v>363</v>
+        <v>763</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B170" t="s">
-        <v>797</v>
+        <v>760</v>
       </c>
       <c r="C170" s="25" t="s">
-        <v>798</v>
+        <v>764</v>
       </c>
       <c r="D170" t="s">
-        <v>799</v>
+        <v>765</v>
       </c>
       <c r="E170" t="s">
-        <v>800</v>
-      </c>
-      <c r="F170" t="s">
-        <v>801</v>
-      </c>
-      <c r="G170" t="s">
-        <v>802</v>
+        <v>766</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B171" t="s">
-        <v>803</v>
+        <v>925</v>
       </c>
       <c r="C171" s="25" t="s">
-        <v>804</v>
+        <v>929</v>
       </c>
       <c r="D171" t="s">
-        <v>805</v>
-      </c>
-      <c r="E171" t="s">
-        <v>806</v>
-      </c>
-      <c r="F171" t="s">
-        <v>807</v>
-      </c>
-      <c r="G171" t="s">
-        <v>363</v>
+        <v>928</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>778</v>
-      </c>
-      <c r="B172" s="31" t="s">
-        <v>803</v>
-      </c>
-      <c r="C172" s="25" t="s">
-        <v>808</v>
+        <v>697</v>
+      </c>
+      <c r="B172" t="s">
+        <v>925</v>
+      </c>
+      <c r="C172" s="48" t="s">
+        <v>926</v>
       </c>
       <c r="D172" t="s">
-        <v>805</v>
-      </c>
-      <c r="E172" t="s">
-        <v>809</v>
+        <v>927</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B173" t="s">
-        <v>810</v>
+        <v>921</v>
       </c>
       <c r="C173" s="25" t="s">
-        <v>811</v>
+        <v>922</v>
       </c>
       <c r="D173" t="s">
-        <v>812</v>
-      </c>
-      <c r="E173" t="s">
-        <v>813</v>
-      </c>
-      <c r="F173" t="s">
-        <v>814</v>
-      </c>
-      <c r="G173" t="s">
-        <v>344</v>
+        <v>924</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B174" t="s">
-        <v>810</v>
+        <v>921</v>
       </c>
       <c r="C174" s="25" t="s">
-        <v>815</v>
+        <v>923</v>
       </c>
       <c r="D174" t="s">
-        <v>816</v>
-      </c>
-      <c r="E174" t="s">
-        <v>817</v>
-      </c>
-      <c r="F174" t="s">
-        <v>818</v>
-      </c>
-      <c r="G174" t="s">
-        <v>344</v>
+        <v>924</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B175" t="s">
-        <v>819</v>
+        <v>921</v>
       </c>
       <c r="C175" s="25" t="s">
-        <v>820</v>
+        <v>964</v>
       </c>
       <c r="D175" t="s">
-        <v>821</v>
-      </c>
-      <c r="E175" t="s">
-        <v>822</v>
-      </c>
-      <c r="F175" t="s">
-        <v>823</v>
-      </c>
-      <c r="G175" t="s">
-        <v>344</v>
+        <v>924</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B176" t="s">
-        <v>824</v>
+        <v>767</v>
       </c>
       <c r="C176" s="25" t="s">
-        <v>825</v>
+        <v>768</v>
       </c>
       <c r="D176" t="s">
-        <v>826</v>
+        <v>769</v>
       </c>
       <c r="E176" t="s">
-        <v>827</v>
-      </c>
-      <c r="F176" t="s">
-        <v>828</v>
-      </c>
-      <c r="G176" t="s">
-        <v>363</v>
+        <v>770</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B177" t="s">
-        <v>829</v>
+        <v>767</v>
       </c>
       <c r="C177" s="25" t="s">
-        <v>830</v>
+        <v>771</v>
       </c>
       <c r="D177" t="s">
-        <v>831</v>
+        <v>769</v>
       </c>
       <c r="E177" t="s">
-        <v>832</v>
-      </c>
-      <c r="F177" t="s">
-        <v>833</v>
-      </c>
-      <c r="G177" t="s">
-        <v>344</v>
+        <v>770</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B178" t="s">
-        <v>829</v>
+        <v>767</v>
       </c>
       <c r="C178" s="25" t="s">
-        <v>834</v>
+        <v>772</v>
       </c>
       <c r="D178" t="s">
-        <v>835</v>
+        <v>773</v>
       </c>
       <c r="E178" t="s">
-        <v>836</v>
-      </c>
-      <c r="F178" t="s">
-        <v>837</v>
-      </c>
-      <c r="G178" t="s">
-        <v>344</v>
+        <v>770</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>778</v>
+        <v>697</v>
       </c>
       <c r="B179" t="s">
-        <v>838</v>
+        <v>774</v>
       </c>
       <c r="C179" s="25" t="s">
-        <v>839</v>
+        <v>775</v>
       </c>
       <c r="D179" t="s">
-        <v>840</v>
+        <v>776</v>
       </c>
       <c r="E179" t="s">
-        <v>841</v>
-      </c>
-      <c r="F179" t="s">
-        <v>842</v>
-      </c>
-      <c r="G179" t="s">
-        <v>363</v>
+        <v>777</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
@@ -8816,13 +8774,22 @@
         <v>778</v>
       </c>
       <c r="B180" t="s">
-        <v>843</v>
+        <v>779</v>
       </c>
       <c r="C180" s="25" t="s">
-        <v>844</v>
+        <v>780</v>
       </c>
       <c r="D180" t="s">
-        <v>845</v>
+        <v>781</v>
+      </c>
+      <c r="E180" t="s">
+        <v>782</v>
+      </c>
+      <c r="F180" t="s">
+        <v>783</v>
+      </c>
+      <c r="G180" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
@@ -8830,19 +8797,19 @@
         <v>778</v>
       </c>
       <c r="B181" t="s">
-        <v>846</v>
+        <v>779</v>
       </c>
       <c r="C181" s="25" t="s">
-        <v>847</v>
+        <v>784</v>
       </c>
       <c r="D181" t="s">
-        <v>848</v>
+        <v>785</v>
       </c>
       <c r="E181" t="s">
-        <v>849</v>
+        <v>786</v>
       </c>
       <c r="F181" t="s">
-        <v>850</v>
+        <v>787</v>
       </c>
       <c r="G181" t="s">
         <v>363</v>
@@ -8853,16 +8820,22 @@
         <v>778</v>
       </c>
       <c r="B182" t="s">
-        <v>851</v>
+        <v>779</v>
       </c>
       <c r="C182" s="25" t="s">
-        <v>852</v>
+        <v>788</v>
       </c>
       <c r="D182" t="s">
-        <v>853</v>
+        <v>789</v>
       </c>
       <c r="E182" t="s">
-        <v>854</v>
+        <v>790</v>
+      </c>
+      <c r="F182" t="s">
+        <v>791</v>
+      </c>
+      <c r="G182" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
@@ -8870,16 +8843,22 @@
         <v>778</v>
       </c>
       <c r="B183" t="s">
-        <v>855</v>
+        <v>792</v>
       </c>
       <c r="C183" s="25" t="s">
-        <v>856</v>
+        <v>340</v>
       </c>
       <c r="D183" t="s">
-        <v>857</v>
+        <v>341</v>
       </c>
       <c r="E183" t="s">
-        <v>858</v>
+        <v>793</v>
+      </c>
+      <c r="F183" t="s">
+        <v>794</v>
+      </c>
+      <c r="G183" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
@@ -8887,16 +8866,22 @@
         <v>778</v>
       </c>
       <c r="B184" t="s">
-        <v>859</v>
+        <v>792</v>
       </c>
       <c r="C184" s="25" t="s">
-        <v>860</v>
+        <v>795</v>
       </c>
       <c r="D184" t="s">
-        <v>861</v>
+        <v>796</v>
       </c>
       <c r="E184" t="s">
-        <v>862</v>
+        <v>793</v>
+      </c>
+      <c r="F184" t="s">
+        <v>794</v>
+      </c>
+      <c r="G184" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
@@ -8904,85 +8889,352 @@
         <v>778</v>
       </c>
       <c r="B185" t="s">
+        <v>797</v>
+      </c>
+      <c r="C185" s="25" t="s">
+        <v>798</v>
+      </c>
+      <c r="D185" t="s">
+        <v>799</v>
+      </c>
+      <c r="E185" t="s">
+        <v>800</v>
+      </c>
+      <c r="F185" t="s">
+        <v>801</v>
+      </c>
+      <c r="G185" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>778</v>
+      </c>
+      <c r="B186" t="s">
+        <v>803</v>
+      </c>
+      <c r="C186" s="25" t="s">
+        <v>804</v>
+      </c>
+      <c r="D186" t="s">
+        <v>805</v>
+      </c>
+      <c r="E186" t="s">
+        <v>806</v>
+      </c>
+      <c r="F186" t="s">
+        <v>807</v>
+      </c>
+      <c r="G186" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>778</v>
+      </c>
+      <c r="B187" s="31" t="s">
+        <v>803</v>
+      </c>
+      <c r="C187" s="25" t="s">
+        <v>808</v>
+      </c>
+      <c r="D187" t="s">
+        <v>805</v>
+      </c>
+      <c r="E187" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>778</v>
+      </c>
+      <c r="B188" t="s">
+        <v>810</v>
+      </c>
+      <c r="C188" s="25" t="s">
+        <v>811</v>
+      </c>
+      <c r="D188" t="s">
+        <v>812</v>
+      </c>
+      <c r="E188" t="s">
+        <v>813</v>
+      </c>
+      <c r="F188" t="s">
+        <v>814</v>
+      </c>
+      <c r="G188" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>778</v>
+      </c>
+      <c r="B189" t="s">
+        <v>810</v>
+      </c>
+      <c r="C189" s="25" t="s">
+        <v>815</v>
+      </c>
+      <c r="D189" t="s">
+        <v>816</v>
+      </c>
+      <c r="E189" t="s">
+        <v>817</v>
+      </c>
+      <c r="F189" t="s">
+        <v>818</v>
+      </c>
+      <c r="G189" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>778</v>
+      </c>
+      <c r="B190" t="s">
+        <v>819</v>
+      </c>
+      <c r="C190" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="D190" t="s">
+        <v>821</v>
+      </c>
+      <c r="E190" t="s">
+        <v>822</v>
+      </c>
+      <c r="F190" t="s">
+        <v>823</v>
+      </c>
+      <c r="G190" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>778</v>
+      </c>
+      <c r="B191" t="s">
+        <v>824</v>
+      </c>
+      <c r="C191" s="25" t="s">
+        <v>825</v>
+      </c>
+      <c r="D191" t="s">
+        <v>826</v>
+      </c>
+      <c r="E191" t="s">
+        <v>827</v>
+      </c>
+      <c r="F191" t="s">
+        <v>828</v>
+      </c>
+      <c r="G191" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>778</v>
+      </c>
+      <c r="B192" t="s">
+        <v>829</v>
+      </c>
+      <c r="C192" s="25" t="s">
+        <v>830</v>
+      </c>
+      <c r="D192" t="s">
+        <v>831</v>
+      </c>
+      <c r="E192" t="s">
+        <v>832</v>
+      </c>
+      <c r="F192" t="s">
+        <v>833</v>
+      </c>
+      <c r="G192" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>778</v>
+      </c>
+      <c r="B193" t="s">
+        <v>829</v>
+      </c>
+      <c r="C193" s="25" t="s">
+        <v>834</v>
+      </c>
+      <c r="D193" t="s">
+        <v>835</v>
+      </c>
+      <c r="E193" t="s">
+        <v>836</v>
+      </c>
+      <c r="F193" t="s">
+        <v>837</v>
+      </c>
+      <c r="G193" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>778</v>
+      </c>
+      <c r="B194" t="s">
+        <v>838</v>
+      </c>
+      <c r="C194" s="25" t="s">
+        <v>839</v>
+      </c>
+      <c r="D194" t="s">
+        <v>840</v>
+      </c>
+      <c r="E194" t="s">
+        <v>841</v>
+      </c>
+      <c r="F194" t="s">
+        <v>842</v>
+      </c>
+      <c r="G194" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>778</v>
+      </c>
+      <c r="B195" t="s">
+        <v>843</v>
+      </c>
+      <c r="C195" s="25" t="s">
+        <v>844</v>
+      </c>
+      <c r="D195" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>778</v>
+      </c>
+      <c r="B196" t="s">
+        <v>846</v>
+      </c>
+      <c r="C196" s="25" t="s">
+        <v>847</v>
+      </c>
+      <c r="D196" t="s">
+        <v>848</v>
+      </c>
+      <c r="E196" t="s">
+        <v>849</v>
+      </c>
+      <c r="F196" t="s">
+        <v>850</v>
+      </c>
+      <c r="G196" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>778</v>
+      </c>
+      <c r="B197" t="s">
+        <v>851</v>
+      </c>
+      <c r="C197" s="25" t="s">
+        <v>852</v>
+      </c>
+      <c r="D197" t="s">
+        <v>853</v>
+      </c>
+      <c r="E197" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>778</v>
+      </c>
+      <c r="B198" t="s">
+        <v>855</v>
+      </c>
+      <c r="C198" s="25" t="s">
+        <v>856</v>
+      </c>
+      <c r="D198" t="s">
+        <v>857</v>
+      </c>
+      <c r="E198" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>778</v>
+      </c>
+      <c r="B199" t="s">
         <v>859</v>
       </c>
-      <c r="C185" s="25" t="s">
+      <c r="C199" s="25" t="s">
+        <v>860</v>
+      </c>
+      <c r="D199" t="s">
+        <v>861</v>
+      </c>
+      <c r="E199" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>778</v>
+      </c>
+      <c r="B200" t="s">
+        <v>859</v>
+      </c>
+      <c r="C200" s="25" t="s">
         <v>863</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D200" t="s">
         <v>861</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E200" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C186"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C187"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C188"/>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C189"/>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C190"/>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C191"/>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C192"/>
-    </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C193"/>
-    </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C194"/>
-    </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C195"/>
-    </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C196"/>
-    </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C197"/>
-    </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C198"/>
-    </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C199"/>
-    </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C200"/>
-    </row>
-    <row r="201" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C201"/>
     </row>
-    <row r="202" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C202"/>
     </row>
-    <row r="203" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C203"/>
     </row>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C204"/>
     </row>
-    <row r="205" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C205"/>
     </row>
-    <row r="206" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C206"/>
     </row>
-    <row r="207" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C207"/>
     </row>
-    <row r="208" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C208"/>
     </row>
     <row r="209" spans="3:3" x14ac:dyDescent="0.2">
@@ -9359,6 +9611,51 @@
     </row>
     <row r="333" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C333"/>
+    </row>
+    <row r="334" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C334"/>
+    </row>
+    <row r="335" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C335"/>
+    </row>
+    <row r="336" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C336"/>
+    </row>
+    <row r="337" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C337"/>
+    </row>
+    <row r="338" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C338"/>
+    </row>
+    <row r="339" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C339"/>
+    </row>
+    <row r="340" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C340"/>
+    </row>
+    <row r="341" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C341"/>
+    </row>
+    <row r="342" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C342"/>
+    </row>
+    <row r="343" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C343"/>
+    </row>
+    <row r="344" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C344"/>
+    </row>
+    <row r="345" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C345"/>
+    </row>
+    <row r="346" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C346"/>
+    </row>
+    <row r="347" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C347"/>
+    </row>
+    <row r="348" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C348"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9366,6 +9663,37 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="0af18bdd-3447-408d-80d3-6f9fce434a6a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="ce57bbcd-944d-48da-b7d9-79b20bf66928">
+      <UserInfo>
+        <DisplayName>Tim Fliss</DisplayName>
+        <AccountId>767</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <Assignee xmlns="0af18bdd-3447-408d-80d3-6f9fce434a6a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Assignee>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005939B070FDF5B144BCD3855A402129DF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="164d5d93613e4479ad941b94e601e051">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0af18bdd-3447-408d-80d3-6f9fce434a6a" xmlns:ns3="ce57bbcd-944d-48da-b7d9-79b20bf66928" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4e9fa8756f89084b8548b8117c2dd74" ns2:_="" ns3:_="">
     <xsd:import namespace="0af18bdd-3447-408d-80d3-6f9fce434a6a"/>
@@ -9616,38 +9944,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77F7C331-08C4-4F14-8B6A-29CD8DF47E6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="0af18bdd-3447-408d-80d3-6f9fce434a6a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="ce57bbcd-944d-48da-b7d9-79b20bf66928">
-      <UserInfo>
-        <DisplayName>Tim Fliss</DisplayName>
-        <AccountId>767</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <Assignee xmlns="0af18bdd-3447-408d-80d3-6f9fce434a6a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Assignee>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8494D3F1-3EF7-4062-8C18-CF37BCAAC176}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0af18bdd-3447-408d-80d3-6f9fce434a6a"/>
+    <ds:schemaRef ds:uri="ce57bbcd-944d-48da-b7d9-79b20bf66928"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{700F0BDA-F005-4B70-B3FA-A086EC97F59F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9664,23 +9980,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77F7C331-08C4-4F14-8B6A-29CD8DF47E6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8494D3F1-3EF7-4062-8C18-CF37BCAAC176}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0af18bdd-3447-408d-80d3-6f9fce434a6a"/>
-    <ds:schemaRef ds:uri="ce57bbcd-944d-48da-b7d9-79b20bf66928"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>